<commit_message>
Fixat resultaten i finrisk lab 3
</commit_message>
<xml_diff>
--- a/finrisk/Lab3/DataLab3Student.xlsx
+++ b/finrisk/Lab3/DataLab3Student.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah\Desktop\Skola\År 4\Finrisk + Monte Carlo\LP32020\LP32020\finrisk\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C027D10-3E1B-40AE-95A4-13C132F26369}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3434C55A-2063-4180-9D2F-14AA70061332}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="2745" windowWidth="19185" windowHeight="10185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -144,11 +144,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000000000000"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
     <numFmt numFmtId="167" formatCode="0.000%"/>
+    <numFmt numFmtId="169" formatCode="0.00000%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -195,7 +196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -209,6 +210,7 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,12 +681,12 @@
         <v>487.07609511363637</v>
       </c>
       <c r="N4" s="11">
-        <f>K20*AVERAGE(B434:B454)/10^9</f>
-        <v>523.14823264285712</v>
-      </c>
-      <c r="O4" s="11">
         <f>K20*AVERAGE(B685:B706)/10^9</f>
         <v>1037.1310872272727</v>
+      </c>
+      <c r="O4" s="11">
+        <f>K20*AVERAGE(B915:B934)/10^9</f>
+        <v>292.77777823000002</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -726,12 +728,12 @@
         <v>3.0047727272727275E-2</v>
       </c>
       <c r="N5" s="10">
-        <f>AVERAGE(H434:H454)</f>
-        <v>3.2314285714285719E-2</v>
-      </c>
-      <c r="O5" s="10">
         <f>AVERAGE(H685:H706)</f>
         <v>3.9831818181818184E-2</v>
+      </c>
+      <c r="O5" s="10">
+        <f>AVERAGE(H915:H934)</f>
+        <v>4.0075E-2</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -761,24 +763,24 @@
         <v>15</v>
       </c>
       <c r="K6" s="11">
-        <f>AVERAGE(E23:E42)/10^9</f>
-        <v>481.12588306643244</v>
+        <f>AVERAGE(E22:E41)/10^9</f>
+        <v>480.8758871641885</v>
       </c>
       <c r="L6" s="11">
-        <f>AVERAGE(E166:E187)/10^9</f>
-        <v>517.12529298955849</v>
+        <f>AVERAGE(E165:E186)/10^9</f>
+        <v>516.87529708731449</v>
       </c>
       <c r="M6" s="11">
-        <f>AVERAGE(E391:E412)/10^9</f>
-        <v>601.84677419354773</v>
+        <f>AVERAGE(E390:E411)/10^9</f>
+        <v>601.41129032258016</v>
       </c>
       <c r="N6" s="11">
-        <f>AVERAGE(E435:E455)/10^9</f>
-        <v>620.79032258064456</v>
+        <f>AVERAGE(E685:E706)/10^9</f>
+        <v>762.7</v>
       </c>
       <c r="O6" s="11">
-        <f>AVERAGE(E686:E707)/10^9</f>
-        <v>763.3</v>
+        <f>AVERAGE(E915:E934)/10^9</f>
+        <v>828.7</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -808,24 +810,24 @@
         <v>16</v>
       </c>
       <c r="K7">
-        <f>_xlfn.STDEV.P(C22:C41)*SQRT(252)/2</f>
-        <v>0.10478604887854083</v>
+        <f>_xlfn.STDEV.S(C22:C41)*SQRT(252)/2</f>
+        <v>0.10750821774991974</v>
       </c>
       <c r="L7">
-        <f>_xlfn.STDEV.P(C165:C186)*SQRT(252)/2</f>
-        <v>0.32173833713029798</v>
+        <f>_xlfn.STDEV.S(C165:C186)*SQRT(252)/2</f>
+        <v>0.32930968683756257</v>
       </c>
       <c r="M7">
-        <f>_xlfn.STDEV.P(C390:C411)*SQRT(252)/2</f>
-        <v>0.16318166367859324</v>
+        <f>_xlfn.STDEV.S(C390:C411)*SQRT(252)/2</f>
+        <v>0.16702175762743315</v>
       </c>
       <c r="N7">
-        <f>_xlfn.STDEV.P(C434:C454)*SQRT(252)/2</f>
-        <v>0.26067694154178905</v>
+        <f>_xlfn.STDEV.S(C685:C706)*SQRT(252)/2</f>
+        <v>0.45397604795181762</v>
       </c>
       <c r="O7">
-        <f>_xlfn.STDEV.P(C685:C706)*SQRT(252)/2</f>
-        <v>0.44353842174417862</v>
+        <f>_xlfn.STDEV.S(C915:C934)*SQRT(252)/2</f>
+        <v>0.45707634618931708</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -855,19 +857,19 @@
         <v>17</v>
       </c>
       <c r="K8" s="11">
-        <v>778.20702036411251</v>
+        <v>777.96762687202784</v>
       </c>
       <c r="L8" s="11">
-        <v>799.01911267643425</v>
+        <v>798.11346549327698</v>
       </c>
       <c r="M8" s="11">
-        <v>1071.1046222616208</v>
+        <v>1070.6806450530303</v>
       </c>
       <c r="N8" s="11">
-        <v>1123.6201436399663</v>
+        <v>1764.9547625728442</v>
       </c>
       <c r="O8" s="11">
-        <v>1766.2046813630648</v>
+        <v>1011.8977793900551</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -898,23 +900,23 @@
       </c>
       <c r="K9">
         <f>(LN(K8/K6) + (K5+(K7^2)/2))/K7</f>
-        <v>5.0550020585898112</v>
+        <v>4.9316668639890393</v>
       </c>
       <c r="L9">
         <f t="shared" ref="L9:O9" si="1">(LN(L8/L6) + (L5+(L7^2)/2))/L7</f>
-        <v>1.6432981031458238</v>
+        <v>1.6110249279187245</v>
       </c>
       <c r="M9">
         <f t="shared" si="1"/>
-        <v>3.7982498044393482</v>
+        <v>3.7166813962727612</v>
       </c>
       <c r="N9">
         <f t="shared" si="1"/>
-        <v>2.5303663548262696</v>
+        <v>2.162877355021616</v>
       </c>
       <c r="O9">
         <f t="shared" si="1"/>
-        <v>2.2030382776672157</v>
+        <v>0.75317619118964341</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -945,23 +947,23 @@
       </c>
       <c r="K10">
         <f>K9-K7</f>
-        <v>4.9502160097112702</v>
+        <v>4.8241586462391197</v>
       </c>
       <c r="L10">
         <f t="shared" ref="L10:O10" si="2">L9-L7</f>
-        <v>1.3215597660155258</v>
+        <v>1.2817152410811619</v>
       </c>
       <c r="M10">
         <f t="shared" si="2"/>
-        <v>3.635068140760755</v>
+        <v>3.5496596386453279</v>
       </c>
       <c r="N10">
         <f t="shared" si="2"/>
-        <v>2.2696894132844805</v>
+        <v>1.7089013070697985</v>
       </c>
       <c r="O10">
         <f t="shared" si="2"/>
-        <v>1.759499855923037</v>
+        <v>0.29609984500032632</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -992,23 +994,23 @@
       </c>
       <c r="K11">
         <f>_xlfn.NORM.S.DIST(K9,TRUE)</f>
-        <v>0.99999978480693685</v>
+        <v>0.99999959234560998</v>
       </c>
       <c r="L11">
         <f t="shared" ref="L11:O11" si="3">_xlfn.NORM.S.DIST(L9,TRUE)</f>
-        <v>0.94983936470710617</v>
+        <v>0.946412855345097</v>
       </c>
       <c r="M11">
         <f t="shared" si="3"/>
-        <v>0.99992713928920463</v>
+        <v>0.99989907163530234</v>
       </c>
       <c r="N11">
         <f t="shared" si="3"/>
-        <v>0.99430282580441287</v>
+        <v>0.98472469304833854</v>
       </c>
       <c r="O11">
         <f t="shared" si="3"/>
-        <v>0.98620397456827325</v>
+        <v>0.77432797775635609</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1039,23 +1041,23 @@
       </c>
       <c r="K12">
         <f>_xlfn.NORM.S.DIST(K10,TRUE)</f>
-        <v>0.99999962934421627</v>
+        <v>0.99999929702260382</v>
       </c>
       <c r="L12">
         <f t="shared" ref="L12:O12" si="4">_xlfn.NORM.S.DIST(L10,TRUE)</f>
-        <v>0.90684260575957765</v>
+        <v>0.90002872177109128</v>
       </c>
       <c r="M12">
         <f t="shared" si="4"/>
-        <v>0.99986104641442997</v>
+        <v>0.99980713524355136</v>
       </c>
       <c r="N12">
         <f t="shared" si="4"/>
-        <v>0.98838678289944559</v>
+        <v>0.95626538381403803</v>
       </c>
       <c r="O12">
         <f t="shared" si="4"/>
-        <v>0.96075367765228503</v>
+        <v>0.61642308382305222</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1086,23 +1088,23 @@
       </c>
       <c r="K13" s="9">
         <f xml:space="preserve"> (K4-(K8*K11-K6*EXP(-K5)*K12))^2</f>
-        <v>5.2249001267542947E-12</v>
+        <v>2.0390798293083457E-18</v>
       </c>
       <c r="L13" s="9">
         <f xml:space="preserve"> (L4-(L8*L11-L6*EXP(-L5)*L12))^2</f>
-        <v>1.7734688323725221E-10</v>
+        <v>1.1432414778481379E-20</v>
       </c>
       <c r="M13" s="9">
         <f t="shared" ref="M13:O13" si="5" xml:space="preserve"> (M4-(M8*M11-M6*EXP(-M5)*M12))^2</f>
-        <v>1.8663262570727687E-23</v>
+        <v>7.680473832099831E-14</v>
       </c>
       <c r="N13" s="9">
         <f t="shared" si="5"/>
-        <v>6.0821847141695564E-18</v>
+        <v>2.4304921522864184E-9</v>
       </c>
       <c r="O13" s="9">
         <f t="shared" si="5"/>
-        <v>7.1754980205404394E-14</v>
+        <v>8.9569310991014915E-9</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1133,23 +1135,23 @@
       </c>
       <c r="K14">
         <f>(LN(K8/K6)+(K5-K7^2/2)/(K8))</f>
-        <v>0.48091227214169296</v>
+        <v>0.48112398756037611</v>
       </c>
       <c r="L14">
         <f t="shared" ref="L14:O14" si="6">(LN(L8/L6)+(L5-L7^2/2)/(L8))</f>
-        <v>0.43508728063292207</v>
+        <v>0.43443363771838639</v>
       </c>
       <c r="M14">
         <f t="shared" si="6"/>
-        <v>0.57645848995198468</v>
+        <v>0.57678583509737813</v>
       </c>
       <c r="N14">
         <f t="shared" si="6"/>
-        <v>0.59331616361480621</v>
+        <v>0.83897975264194546</v>
       </c>
       <c r="O14">
         <f t="shared" si="6"/>
-        <v>0.83890399713753538</v>
+        <v>0.19966100101413389</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1180,23 +1182,23 @@
       </c>
       <c r="K15">
         <f>_xlfn.NORM.S.DIST(-K14,TRUE)</f>
-        <v>0.31528942514286362</v>
+        <v>0.31521419024031416</v>
       </c>
       <c r="L15">
         <f>_xlfn.NORM.S.DIST(-L14,TRUE)</f>
-        <v>0.33174953774186294</v>
+        <v>0.33198678771494489</v>
       </c>
       <c r="M15">
         <f>_xlfn.NORM.S.DIST(-M14,TRUE)</f>
-        <v>0.28215265981056215</v>
+        <v>0.28204206977292512</v>
       </c>
       <c r="N15">
         <f>_xlfn.NORM.S.DIST(-N14,TRUE)</f>
-        <v>0.27648479172801055</v>
+        <v>0.20074033583886983</v>
       </c>
       <c r="O15">
         <f>_xlfn.NORM.S.DIST(-O14,TRUE)</f>
-        <v>0.20076159229865853</v>
+        <v>0.42087285812902225</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1227,23 +1229,23 @@
       </c>
       <c r="K16" s="12">
         <f>(LN(K6)-LN(K8-K4))-K5</f>
-        <v>1.2131729093534105E-8</v>
+        <v>1.4260058606163639E-8</v>
       </c>
       <c r="L16" s="12">
         <f>(LN(L6)-LN(L8-L4))-L5</f>
-        <v>1.24174056446388E-2</v>
-      </c>
-      <c r="M16" s="12">
+        <v>1.378455082097476E-2</v>
+      </c>
+      <c r="M16" s="13">
         <f>(LN(M6)-LN(M8-M4))-M5</f>
-        <v>5.3282293242321033E-6</v>
+        <v>7.7035548791473674E-6</v>
       </c>
       <c r="N16" s="12">
         <f>(LN(N6)-LN(N8-N4))-N5</f>
-        <v>9.6323000547184762E-4</v>
+        <v>6.9741363235054712E-3</v>
       </c>
       <c r="O16" s="12">
         <f>(LN(O6)-LN(O8-O4))-O5</f>
-        <v>6.0446415339786078E-3</v>
+        <v>0.10175496397669356</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -24786,6 +24788,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100E825780FFF0FDF43AF9E88D3D0DD3F64" ma:contentTypeVersion="2" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="85bd80a5e468ea5561f0835e87691bea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8d973635-663e-44ce-8d6c-70fd171f495a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7cf3fc15204a56ef9345b094e583ba4b" ns2:_="">
     <xsd:import namespace="8d973635-663e-44ce-8d6c-70fd171f495a"/>
@@ -24917,12 +24925,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -24933,6 +24935,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{449188B4-4BDF-450B-8953-4DEA7D9AB904}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8d973635-663e-44ce-8d6c-70fd171f495a"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0C5AD0-5984-468E-A604-7F6BE591EFAF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24950,22 +24968,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{449188B4-4BDF-450B-8953-4DEA7D9AB904}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8d973635-663e-44ce-8d6c-70fd171f495a"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF15EFC-AC7F-42BC-85CA-1DE95B4D8D94}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fixat excel för finrisk
</commit_message>
<xml_diff>
--- a/finrisk/Lab3/DataLab3Student.xlsx
+++ b/finrisk/Lab3/DataLab3Student.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah\Desktop\Skola\År 4\Finrisk + Monte Carlo\LP32020\LP32020\finrisk\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3434C55A-2063-4180-9D2F-14AA70061332}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3262889A-8671-4506-81FB-E198FB5C8AA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,9 +113,6 @@
     <t>$r_f$</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>$\sigma_A$</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   <si>
     <t xml:space="preserve"> Oct 01</t>
   </si>
+  <si>
+    <t>K</t>
+  </si>
 </sst>
 </file>
 
@@ -149,7 +149,7 @@
     <numFmt numFmtId="165" formatCode="0.00000000000000"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
     <numFmt numFmtId="167" formatCode="0.000%"/>
-    <numFmt numFmtId="169" formatCode="0.00000%"/>
+    <numFmt numFmtId="168" formatCode="0.00000%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -210,7 +210,7 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,7 +553,7 @@
   <dimension ref="A1:O996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,19 +603,19 @@
       </c>
       <c r="I2" s="8"/>
       <c r="K2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" t="s">
         <v>22</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -760,7 +760,7 @@
         <v>4.4800000000000006E-2</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="K6" s="11">
         <f>AVERAGE(E22:E41)/10^9</f>
@@ -807,7 +807,7 @@
         <v>4.4299999999999999E-2</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K7">
         <f>_xlfn.STDEV.S(C22:C41)*SQRT(252)/2</f>
@@ -854,7 +854,7 @@
         <v>4.4400000000000002E-2</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K8" s="11">
         <v>777.96762687202784</v>
@@ -1084,7 +1084,7 @@
         <v>4.41E-2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K13" s="9">
         <f xml:space="preserve"> (K4-(K8*K11-K6*EXP(-K5)*K12))^2</f>
@@ -1134,24 +1134,24 @@
         <v>5</v>
       </c>
       <c r="K14">
-        <f>(LN(K8/K6)+(K5-K7^2/2)/(K8))</f>
-        <v>0.48112398756037611</v>
+        <f>(LN(K8/K6)+(K5-(K7^2)/2))/(K7)</f>
+        <v>4.8241586462391197</v>
       </c>
       <c r="L14">
-        <f t="shared" ref="L14:O14" si="6">(LN(L8/L6)+(L5-L7^2/2)/(L8))</f>
-        <v>0.43443363771838639</v>
+        <f t="shared" ref="L14:O14" si="6">(LN(L8/L6)+(L5-(L7^2)/2))/(L7)</f>
+        <v>1.2817152410811619</v>
       </c>
       <c r="M14">
         <f t="shared" si="6"/>
-        <v>0.57678583509737813</v>
+        <v>3.5496596386453283</v>
       </c>
       <c r="N14">
         <f t="shared" si="6"/>
-        <v>0.83897975264194546</v>
+        <v>1.7089013070697985</v>
       </c>
       <c r="O14">
         <f t="shared" si="6"/>
-        <v>0.19966100101413389</v>
+        <v>0.29609984500032638</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1180,25 +1180,25 @@
       <c r="J15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="10">
         <f>_xlfn.NORM.S.DIST(-K14,TRUE)</f>
-        <v>0.31521419024031416</v>
-      </c>
-      <c r="L15">
+        <v>7.0297739612883502E-7</v>
+      </c>
+      <c r="L15" s="10">
         <f>_xlfn.NORM.S.DIST(-L14,TRUE)</f>
-        <v>0.33198678771494489</v>
-      </c>
-      <c r="M15">
+        <v>9.9971278228908694E-2</v>
+      </c>
+      <c r="M15" s="10">
         <f>_xlfn.NORM.S.DIST(-M14,TRUE)</f>
-        <v>0.28204206977292512</v>
-      </c>
-      <c r="N15">
+        <v>1.9286475644868779E-4</v>
+      </c>
+      <c r="N15" s="10">
         <f>_xlfn.NORM.S.DIST(-N14,TRUE)</f>
-        <v>0.20074033583886983</v>
-      </c>
-      <c r="O15">
+        <v>4.3734616185961944E-2</v>
+      </c>
+      <c r="O15" s="10">
         <f>_xlfn.NORM.S.DIST(-O14,TRUE)</f>
-        <v>0.42087285812902225</v>
+        <v>0.38357691617694772</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -24788,12 +24788,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100E825780FFF0FDF43AF9E88D3D0DD3F64" ma:contentTypeVersion="2" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="85bd80a5e468ea5561f0835e87691bea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8d973635-663e-44ce-8d6c-70fd171f495a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7cf3fc15204a56ef9345b094e583ba4b" ns2:_="">
     <xsd:import namespace="8d973635-663e-44ce-8d6c-70fd171f495a"/>
@@ -24925,6 +24919,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -24935,22 +24935,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{449188B4-4BDF-450B-8953-4DEA7D9AB904}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8d973635-663e-44ce-8d6c-70fd171f495a"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0C5AD0-5984-468E-A604-7F6BE591EFAF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24968,6 +24952,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{449188B4-4BDF-450B-8953-4DEA7D9AB904}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8d973635-663e-44ce-8d6c-70fd171f495a"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF15EFC-AC7F-42BC-85CA-1DE95B4D8D94}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Klar med lab3 Finrisk
</commit_message>
<xml_diff>
--- a/finrisk/Lab3/DataLab3Student.xlsx
+++ b/finrisk/Lab3/DataLab3Student.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah\Desktop\Skola\År 4\Finrisk + Monte Carlo\LP32020\LP32020\finrisk\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3262889A-8671-4506-81FB-E198FB5C8AA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C71F3B5-9CBC-426A-87F7-54D39BEE4A80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>SHARE PRICE ERICSSON B  (SEK)</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>K</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -553,7 +556,7 @@
   <dimension ref="A1:O996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,6 +605,9 @@
         <v>4.3799999999999999E-2</v>
       </c>
       <c r="I2" s="8"/>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
       <c r="K2" s="6" t="s">
         <v>20</v>
       </c>
@@ -24788,6 +24794,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100E825780FFF0FDF43AF9E88D3D0DD3F64" ma:contentTypeVersion="2" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="85bd80a5e468ea5561f0835e87691bea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8d973635-663e-44ce-8d6c-70fd171f495a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7cf3fc15204a56ef9345b094e583ba4b" ns2:_="">
     <xsd:import namespace="8d973635-663e-44ce-8d6c-70fd171f495a"/>
@@ -24919,12 +24931,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -24935,6 +24941,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{449188B4-4BDF-450B-8953-4DEA7D9AB904}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8d973635-663e-44ce-8d6c-70fd171f495a"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0C5AD0-5984-468E-A604-7F6BE591EFAF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24952,22 +24974,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{449188B4-4BDF-450B-8953-4DEA7D9AB904}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8d973635-663e-44ce-8d6c-70fd171f495a"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF15EFC-AC7F-42BC-85CA-1DE95B4D8D94}">
   <ds:schemaRefs>

</xml_diff>